<commit_message>
Fix annex 2 issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_2_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_2_2022.xlsx
@@ -441,7 +441,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>7700</v>
+        <v>15400</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -482,7 +482,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>3300</v>
+        <v>6600</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -523,7 +523,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="H4">
         <v>36000</v>
@@ -564,7 +564,7 @@
         <v>annuelle</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="H5">
         <v>90000</v>
@@ -605,7 +605,7 @@
         <v>annuelle</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="H6">
         <v>90000</v>
@@ -687,7 +687,7 @@
         <v>annuelle</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="H8">
         <v>180000</v>
@@ -728,7 +728,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="H9">
         <v>30000</v>
@@ -769,7 +769,7 @@
         <v>trimestrielle</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="H10">
         <v>60000</v>

</xml_diff>